<commit_message>
Add missing field to spreadsheet
Rcvd Date should also be used for bankstatementsreceived.

Note that this also updates the source_conditions field for
all tables, as the default is now set to a dict rather than
left as the empty string when not specified.
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Reporting.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Reporting.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliotsmith/projects/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliotsmith/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A74641-3BCC-8A46-A86B-968C143A0453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF42EBE-7F44-5D4F-9EEA-32357D5FF111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28820" yWindow="460" windowWidth="38380" windowHeight="19440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28820" yWindow="460" windowWidth="38380" windowHeight="19440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="6" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="119">
   <si>
     <t>table_name</t>
   </si>
@@ -360,14 +360,6 @@
 Sent4
 Sent5
 Sent6</t>
-  </si>
-  <si>
-    <t>Rcvd Date1
-Rcvd Date2
-Rcvd Date3
-Rcvd Date4
-Rcvd Date5
-Rcvd Date6</t>
   </si>
   <si>
     <t>is_at_least_one_set</t>
@@ -825,13 +817,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE371035-1C42-914F-8247-28923EC5B10E}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
     <col min="4" max="4" width="29.1640625" customWidth="1"/>
+    <col min="7" max="7" width="17.83203125" customWidth="1"/>
+    <col min="8" max="8" width="26.1640625" customWidth="1"/>
+    <col min="9" max="9" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.15">
@@ -859,7 +855,7 @@
       <c r="H1" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="I1" s="17"/>
+      <c r="I1" s="16"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="18" t="s">
@@ -910,7 +906,7 @@
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1029,7 +1025,7 @@
       </c>
       <c r="I2" s="26"/>
       <c r="R2" s="17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1060,14 +1056,14 @@
         <v>25</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P3" s="26"/>
       <c r="R3" s="17" t="s">
         <v>94</v>
       </c>
       <c r="S3" s="26" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1174,7 +1170,7 @@
       <c r="H7" s="27"/>
       <c r="I7" s="28"/>
       <c r="R7" s="17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1202,7 +1198,7 @@
       <c r="M8" s="9"/>
       <c r="P8" s="26"/>
       <c r="R8" s="17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S8" s="26"/>
     </row>
@@ -1234,14 +1230,14 @@
         <v>25</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P9" s="26"/>
       <c r="R9" s="17" t="s">
         <v>94</v>
       </c>
       <c r="S9" s="26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1271,7 +1267,7 @@
       </c>
       <c r="I10" s="28"/>
       <c r="R10" s="17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1293,10 +1289,10 @@
       <c r="H11" s="27"/>
       <c r="I11" s="26"/>
       <c r="R11" s="17" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="12" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" ht="99" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>17</v>
       </c>
@@ -1346,7 +1342,7 @@
       <c r="H13" s="27"/>
       <c r="I13" s="26"/>
       <c r="R13" s="17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1368,7 +1364,7 @@
       <c r="H14" s="27"/>
       <c r="I14" s="26"/>
       <c r="R14" s="17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1390,7 +1386,7 @@
       <c r="H15" s="27"/>
       <c r="I15" s="26"/>
       <c r="R15" s="17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1444,7 +1440,7 @@
       <c r="H17" s="27"/>
       <c r="I17" s="26"/>
       <c r="R17" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1466,7 +1462,7 @@
       <c r="H18" s="27"/>
       <c r="I18" s="26"/>
       <c r="R18" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1488,7 +1484,7 @@
       <c r="H19" s="27"/>
       <c r="I19" s="26"/>
       <c r="R19" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1512,7 +1508,7 @@
       <c r="J20" s="9"/>
       <c r="L20" s="29"/>
       <c r="R20" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1537,7 +1533,7 @@
       <c r="H21" s="27"/>
       <c r="I21" s="26"/>
       <c r="R21" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1567,7 +1563,7 @@
         <v>2</v>
       </c>
       <c r="R22" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="S22" s="9" t="s">
         <v>54</v>
@@ -5695,7 +5691,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5798,7 +5794,7 @@
         <v>1</v>
       </c>
       <c r="P2" s="18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5821,7 +5817,7 @@
         <v>57</v>
       </c>
       <c r="P3" s="18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5841,7 +5837,7 @@
         <v>0</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5890,7 +5886,7 @@
         <v>0</v>
       </c>
       <c r="P6" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5949,7 +5945,7 @@
       </c>
       <c r="Q8" s="6"/>
     </row>
-    <row r="9" spans="1:26" ht="85" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" ht="99" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>55</v>
       </c>
@@ -5969,16 +5965,16 @@
         <v>61</v>
       </c>
       <c r="J9" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="K9" t="s">
         <v>108</v>
-      </c>
-      <c r="K9" t="s">
-        <v>109</v>
       </c>
       <c r="P9" s="6" t="s">
         <v>94</v>
       </c>
       <c r="Q9" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5998,7 +5994,7 @@
         <v>0</v>
       </c>
       <c r="P10" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q10" s="6"/>
     </row>
@@ -6031,7 +6027,7 @@
         <v>94</v>
       </c>
       <c r="Q11" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6057,7 +6053,7 @@
         <v>2</v>
       </c>
       <c r="P12" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Q12" s="6" t="s">
         <v>54</v>
@@ -7480,7 +7476,7 @@
   </sheetPr>
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -8529,7 +8525,7 @@
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8565,7 +8561,7 @@
         <v>80</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8593,7 +8589,7 @@
         <v>80</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Add table_transforms for annual_report_logs and annual_report_lodging_details
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Reporting.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Reporting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliotsmith/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF42EBE-7F44-5D4F-9EEA-32357D5FF111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5BA3507-2ABB-5D42-ADD5-5FA768253F9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28820" yWindow="460" windowWidth="38380" windowHeight="19440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="122">
   <si>
     <t>table_name</t>
   </si>
@@ -393,6 +393,15 @@
   </si>
   <si>
     <t>REVIEWED</t>
+  </si>
+  <si>
+    <t>table_transforms</t>
+  </si>
+  <si>
+    <t>set_annual_report_logs_status = {"source_cols": ["Rev Stat", "End Date", "Rcvd Date", "Rcvd Date1", "Rcvd Date2", "Rcvd Date3", "Rcvd Date4", "Rcvd Date5", "Rcvd Date6", "Review Date", "Next Yr"], "target_cols": ["status", "reviewstatus"]}</t>
+  </si>
+  <si>
+    <t>set_annual_report_lodging_details_status = {"source_cols": ["Rev Stat", "End Date", "Rcvd Date", "Rcvd Date1", "Rcvd Date2", "Rcvd Date3", "Rcvd Date4", "Rcvd Date5", "Rcvd Date6", "Review Date", "Next Yr", "Revise Date", "Further Code", "Sent1", "Sent2", "Sent3", "Sent4", "Sent5", "Sent6", "Followup Date"], "target_cols": ["lodgedstatus"]}</t>
   </si>
 </sst>
 </file>
@@ -855,7 +864,9 @@
       <c r="H1" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="I1" s="16"/>
+      <c r="I1" s="16" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="18" t="s">
@@ -876,6 +887,9 @@
       <c r="H2" s="18" t="s">
         <v>104</v>
       </c>
+      <c r="I2" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
@@ -892,6 +906,9 @@
       </c>
       <c r="F3" s="18" t="s">
         <v>105</v>
+      </c>
+      <c r="I3" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -5691,7 +5708,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J11" sqref="J11"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Base implementation for annual_report_logs table transforms
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Reporting.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Reporting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliotsmith/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5BA3507-2ABB-5D42-ADD5-5FA768253F9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0FA55B6-E5FE-0F40-944D-D765B857C1B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28820" yWindow="460" windowWidth="38380" windowHeight="19440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28820" yWindow="460" windowWidth="38380" windowHeight="19440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="6" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="121">
   <si>
     <t>table_name</t>
   </si>
@@ -157,12 +157,6 @@
   </si>
   <si>
     <t>reviewstatus</t>
-  </si>
-  <si>
-    <t>Rev Stat</t>
-  </si>
-  <si>
-    <t>revstatus_lookup</t>
   </si>
   <si>
     <t>reasonforreviewstatuschange</t>
@@ -398,10 +392,13 @@
     <t>table_transforms</t>
   </si>
   <si>
-    <t>set_annual_report_logs_status = {"source_cols": ["Rev Stat", "End Date", "Rcvd Date", "Rcvd Date1", "Rcvd Date2", "Rcvd Date3", "Rcvd Date4", "Rcvd Date5", "Rcvd Date6", "Review Date", "Next Yr"], "target_cols": ["status", "reviewstatus"]}</t>
-  </si>
-  <si>
-    <t>set_annual_report_lodging_details_status = {"source_cols": ["Rev Stat", "End Date", "Rcvd Date", "Rcvd Date1", "Rcvd Date2", "Rcvd Date3", "Rcvd Date4", "Rcvd Date5", "Rcvd Date6", "Review Date", "Next Yr", "Revise Date", "Further Code", "Sent1", "Sent2", "Sent3", "Sent4", "Sent5", "Sent6", "Followup Date"], "target_cols": ["lodgedstatus"]}</t>
+    <t>set_annual_report_lodging_details_status = {"source_cols": ["Rev Stat", "End Date", "Lodge Date", "Rcvd Date", "Rcvd Date1", "Rcvd Date2", "Rcvd Date3", "Rcvd Date4", "Rcvd Date5", "Rcvd Date6", "Review Date", "Next Yr", "Revise Date", "Further Code", "Sent1", "Sent2", "Sent3", "Sent4", "Sent5", "Sent6", "Followup Date"], "target_cols": ["lodgedstatus"]}</t>
+  </si>
+  <si>
+    <t>set_annual_report_logs_status = {"source_cols": ["Rev Stat", "End Date", "Lodge Date", "Rcvd Date", "Rcvd Date1", "Rcvd Date2", "Rcvd Date3", "Rcvd Date4", "Rcvd Date5", "Rcvd Date6", "Review Date", "Next Yr"], "target_cols": ["status", "reviewstatus"]}</t>
+  </si>
+  <si>
+    <t>Mapped by table transform</t>
   </si>
 </sst>
 </file>
@@ -826,8 +823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE371035-1C42-914F-8247-28923EC5B10E}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView topLeftCell="H1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -841,31 +838,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="D1" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="E1" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="F1" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="G1" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="H1" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="G1" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>102</v>
-      </c>
       <c r="I1" s="16" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
@@ -879,36 +876,36 @@
         <v>17</v>
       </c>
       <c r="E2" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="F2" s="18" t="s">
-        <v>105</v>
-      </c>
       <c r="H2" s="18" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E3" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="F3" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="F3" s="18" t="s">
-        <v>105</v>
-      </c>
       <c r="I3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -921,9 +918,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB1000"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1042,7 +1039,7 @@
       </c>
       <c r="I2" s="26"/>
       <c r="R2" s="17" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1073,14 +1070,14 @@
         <v>25</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="P3" s="26"/>
       <c r="R3" s="17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="S3" s="26" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1109,7 +1106,7 @@
       </c>
       <c r="P4" s="26"/>
       <c r="R4" s="17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1137,7 +1134,7 @@
         <v>28</v>
       </c>
       <c r="R5" s="17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1162,7 +1159,7 @@
         <v>0</v>
       </c>
       <c r="R6" s="26" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1187,7 +1184,7 @@
       <c r="H7" s="27"/>
       <c r="I7" s="28"/>
       <c r="R7" s="17" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1215,7 +1212,7 @@
       <c r="M8" s="9"/>
       <c r="P8" s="26"/>
       <c r="R8" s="17" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="S8" s="26"/>
     </row>
@@ -1247,14 +1244,14 @@
         <v>25</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P9" s="26"/>
       <c r="R9" s="17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="S9" s="26" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1284,7 +1281,7 @@
       </c>
       <c r="I10" s="28"/>
       <c r="R10" s="17" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1306,7 +1303,10 @@
       <c r="H11" s="27"/>
       <c r="I11" s="26"/>
       <c r="R11" s="17" t="s">
-        <v>111</v>
+        <v>109</v>
+      </c>
+      <c r="S11" s="17" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:28" ht="99" x14ac:dyDescent="0.2">
@@ -1331,13 +1331,13 @@
         <v>24</v>
       </c>
       <c r="L12" s="15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="M12" s="17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="R12" s="17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1359,7 +1359,7 @@
       <c r="H13" s="27"/>
       <c r="I13" s="26"/>
       <c r="R13" s="17" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1381,7 +1381,7 @@
       <c r="H14" s="27"/>
       <c r="I14" s="26"/>
       <c r="R14" s="17" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1403,7 +1403,7 @@
       <c r="H15" s="27"/>
       <c r="I15" s="26"/>
       <c r="R15" s="17" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1424,19 +1424,15 @@
       </c>
       <c r="H16" s="27"/>
       <c r="I16" s="26"/>
-      <c r="J16" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="L16" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="N16" s="9" t="s">
-        <v>45</v>
-      </c>
+      <c r="J16" s="9"/>
+      <c r="L16" s="7"/>
+      <c r="N16" s="9"/>
       <c r="R16" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="S16" s="9"/>
+        <v>109</v>
+      </c>
+      <c r="S16" s="9" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="17" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
@@ -1446,7 +1442,7 @@
         <v>18</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>38</v>
@@ -1457,7 +1453,7 @@
       <c r="H17" s="27"/>
       <c r="I17" s="26"/>
       <c r="R17" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1468,7 +1464,7 @@
         <v>18</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>38</v>
@@ -1479,7 +1475,7 @@
       <c r="H18" s="27"/>
       <c r="I18" s="26"/>
       <c r="R18" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1490,7 +1486,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>38</v>
@@ -1501,7 +1497,7 @@
       <c r="H19" s="27"/>
       <c r="I19" s="26"/>
       <c r="R19" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1512,7 +1508,7 @@
         <v>18</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>23</v>
@@ -1525,7 +1521,7 @@
       <c r="J20" s="9"/>
       <c r="L20" s="29"/>
       <c r="R20" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1536,7 +1532,7 @@
         <v>18</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>20</v>
@@ -1545,12 +1541,12 @@
         <v>0</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H21" s="27"/>
       <c r="I21" s="26"/>
       <c r="R21" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1561,7 +1557,7 @@
         <v>18</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>20</v>
@@ -1570,20 +1566,20 @@
         <v>0</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H22" s="27"/>
       <c r="I22" s="26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="O22" s="17">
         <v>2</v>
       </c>
       <c r="R22" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="S22" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5796,7 +5792,7 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>18</v>
@@ -5811,18 +5807,18 @@
         <v>1</v>
       </c>
       <c r="P2" s="18" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>20</v>
@@ -5831,41 +5827,41 @@
         <v>0</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="P3" s="18" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E4" s="5" t="b">
         <v>0</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>23</v>
@@ -5874,27 +5870,27 @@
         <v>0</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J5" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q5" s="6" t="s">
         <v>62</v>
-      </c>
-      <c r="P5" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q5" s="6" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>38</v>
@@ -5903,18 +5899,18 @@
         <v>0</v>
       </c>
       <c r="P6" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>23</v>
@@ -5923,24 +5919,24 @@
         <v>0</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="P7" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>38</v>
@@ -5949,60 +5945,60 @@
         <v>0</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="P8" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="Q8" s="6"/>
     </row>
     <row r="9" spans="1:26" ht="99" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E9" s="5" t="b">
         <v>0</v>
       </c>
       <c r="H9" s="20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J9" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="K9" t="s">
         <v>106</v>
       </c>
-      <c r="K9" t="s">
+      <c r="P9" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q9" s="6" t="s">
         <v>108</v>
-      </c>
-      <c r="P9" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q9" s="6" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>23</v>
@@ -6011,19 +6007,19 @@
         <v>0</v>
       </c>
       <c r="P10" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="Q10" s="6"/>
     </row>
     <row r="11" spans="1:26" ht="85" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>23</v>
@@ -6032,30 +6028,30 @@
         <v>0</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J11" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="K11" t="s">
+        <v>91</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q11" s="6" t="s">
         <v>107</v>
-      </c>
-      <c r="K11" t="s">
-        <v>93</v>
-      </c>
-      <c r="P11" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q11" s="6" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>20</v>
@@ -6064,16 +6060,16 @@
         <v>0</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="M12">
         <v>2</v>
       </c>
       <c r="P12" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="Q12" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7502,16 +7498,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7520,10 +7516,10 @@
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8555,105 +8551,105 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="31" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B1" s="31" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D1" s="31" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B2" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="26" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B3" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="26" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B4" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="26" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B5" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D5" s="26"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="26" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B6" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D6" s="26"/>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="26" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B7" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D7" s="26"/>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="26" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B8" s="26" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D8" s="26"/>
     </row>
@@ -9748,7 +9744,7 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>18</v>
@@ -9765,13 +9761,13 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>38</v>
@@ -9782,13 +9778,13 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>38</v>
@@ -9799,13 +9795,13 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>38</v>
@@ -9816,13 +9812,13 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>20</v>
@@ -9831,7 +9827,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Remove unused columns from table transform parameters
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Reporting.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Reporting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliotsmith/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0FA55B6-E5FE-0F40-944D-D765B857C1B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4F17CE-D68B-034B-83E8-46B47DD8369B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28820" yWindow="460" windowWidth="38380" windowHeight="19440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28820" yWindow="460" windowWidth="38380" windowHeight="19440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="6" r:id="rId1"/>
@@ -392,13 +392,13 @@
     <t>table_transforms</t>
   </si>
   <si>
-    <t>set_annual_report_lodging_details_status = {"source_cols": ["Rev Stat", "End Date", "Lodge Date", "Rcvd Date", "Rcvd Date1", "Rcvd Date2", "Rcvd Date3", "Rcvd Date4", "Rcvd Date5", "Rcvd Date6", "Review Date", "Next Yr", "Revise Date", "Further Code", "Sent1", "Sent2", "Sent3", "Sent4", "Sent5", "Sent6", "Followup Date"], "target_cols": ["lodgedstatus"]}</t>
-  </si>
-  <si>
     <t>set_annual_report_logs_status = {"source_cols": ["Rev Stat", "End Date", "Lodge Date", "Rcvd Date", "Rcvd Date1", "Rcvd Date2", "Rcvd Date3", "Rcvd Date4", "Rcvd Date5", "Rcvd Date6", "Review Date", "Next Yr"], "target_cols": ["status", "reviewstatus"]}</t>
   </si>
   <si>
     <t>Mapped by table transform</t>
+  </si>
+  <si>
+    <t>set_annual_report_lodging_details_status = {"source_cols": ["Rev Stat", "Lodge Date", "Rcvd Date", "Rcvd Date1", "Rcvd Date2", "Rcvd Date3", "Rcvd Date4", "Rcvd Date5", "Rcvd Date6", "Review Date", "Revise Date", "Further Code", "Sent1", "Sent2", "Sent3", "Sent4", "Sent5", "Sent6", "Followup Date"], "target_cols": ["lodgedstatus"]}</t>
   </si>
 </sst>
 </file>
@@ -823,8 +823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE371035-1C42-914F-8247-28923EC5B10E}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -885,7 +885,7 @@
         <v>102</v>
       </c>
       <c r="I2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
@@ -905,7 +905,7 @@
         <v>103</v>
       </c>
       <c r="I3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -918,7 +918,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="S16" sqref="S16"/>
     </sheetView>
@@ -1306,7 +1306,7 @@
         <v>109</v>
       </c>
       <c r="S11" s="17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:28" ht="99" x14ac:dyDescent="0.2">
@@ -1431,7 +1431,7 @@
         <v>109</v>
       </c>
       <c r="S16" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add order_id to annual_report_logs migration and add report type assignment
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Reporting.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Reporting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliotsmith/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5A2A6A-1E1B-9240-A672-EDA6392096F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{706CFBF7-D507-9B43-8662-AD13B4E8BA29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28820" yWindow="460" windowWidth="38380" windowHeight="19440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="460" windowWidth="38240" windowHeight="19440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="6" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="106">
   <si>
     <t>table_name</t>
   </si>
@@ -343,6 +343,15 @@
   </si>
   <si>
     <t>set_annual_report_lodging_details_status = {"source_cols": ["Rev Stat", "Lodge Date", "Rcvd Date", "Rcvd Date1", "Rcvd Date2", "Rcvd Date3", "Rcvd Date4", "Rcvd Date5", "Rcvd Date6", "Review Date", "Revise Date", "Further Code", "Sent1", "Sent2", "Sent3", "Sent4", "Sent5", "Sent6", "Followup Date"], "target_cols": ["lodgedstatus"]}</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>As this table has to be derived from a Sirius table joined to a casrec table, any transforms etc. applied in its tab are ignored</t>
+  </si>
+  <si>
+    <t>Mapped during main transform</t>
   </si>
 </sst>
 </file>
@@ -473,7 +482,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -526,6 +535,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -741,22 +751,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE371035-1C42-914F-8247-28923EC5B10E}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView topLeftCell="D1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="27.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.1640625" customWidth="1"/>
     <col min="7" max="7" width="17.83203125" customWidth="1"/>
     <col min="8" max="8" width="26.1640625" customWidth="1"/>
     <col min="9" max="9" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>77</v>
       </c>
@@ -784,8 +794,11 @@
       <c r="I1" s="11" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="J1" s="26" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" s="13" t="s">
         <v>17</v>
       </c>
@@ -808,7 +821,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -826,6 +839,27 @@
       </c>
       <c r="I3" t="s">
         <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A4" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="H4" s="13"/>
+      <c r="J4" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -838,9 +872,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB1000"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S16" sqref="S16"/>
+      <selection pane="bottomLeft" activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1223,7 +1257,7 @@
       <c r="H11" s="22"/>
       <c r="I11" s="21"/>
       <c r="R11" s="12" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="S11" s="12" t="s">
         <v>101</v>
@@ -1348,7 +1382,7 @@
       <c r="L16" s="7"/>
       <c r="N16" s="9"/>
       <c r="R16" s="9" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="S16" s="9" t="s">
         <v>101</v>
@@ -1464,9 +1498,14 @@
         <v>49</v>
       </c>
       <c r="H21" s="22"/>
-      <c r="I21" s="21"/>
+      <c r="I21" s="21" t="s">
+        <v>49</v>
+      </c>
       <c r="R21" s="9" t="s">
-        <v>93</v>
+        <v>76</v>
+      </c>
+      <c r="S21" s="21" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -7402,9 +7441,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7419,7 +7458,7 @@
     <col min="8" max="8" width="12" customWidth="1"/>
     <col min="9" max="9" width="19.83203125" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
-    <col min="11" max="11" width="22.5" customWidth="1"/>
+    <col min="11" max="11" width="24.5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.5" customWidth="1"/>
     <col min="13" max="13" width="13" customWidth="1"/>
     <col min="14" max="14" width="10" customWidth="1"/>
@@ -7506,8 +7545,11 @@
       <c r="E2" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>70</v>
       </c>
@@ -7522,6 +7564,12 @@
       </c>
       <c r="E3" s="5" t="b">
         <v>0</v>
+      </c>
+      <c r="H3" s="13"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="13"/>
+      <c r="P3" s="13" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -7540,6 +7588,9 @@
       <c r="E4" s="5" t="b">
         <v>0</v>
       </c>
+      <c r="P4" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
@@ -7557,6 +7608,9 @@
       <c r="E5" s="5" t="b">
         <v>0</v>
       </c>
+      <c r="P5" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
@@ -7576,6 +7630,9 @@
       </c>
       <c r="G6" s="5" t="s">
         <v>55</v>
+      </c>
+      <c r="P6" s="13" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Set assignee_id to migration user for reporting entity
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Reporting.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Reporting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliotsmith/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A83CF8-7E70-3144-A410-B20F86A76D8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26063C6A-E4E9-DD44-820F-F7491F531844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28820" yWindow="460" windowWidth="38380" windowHeight="19440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28820" yWindow="460" windowWidth="38380" windowHeight="19440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="6" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="103">
   <si>
     <t>table_name</t>
   </si>
@@ -184,9 +184,6 @@
   </si>
   <si>
     <t>assignees:id</t>
-  </si>
-  <si>
-    <t>Add migration user</t>
   </si>
   <si>
     <t>annual_report_lodging_details</t>
@@ -323,9 +320,6 @@
     <t>not mapped</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>calculate_duedate</t>
   </si>
   <si>
@@ -351,6 +345,9 @@
   </si>
   <si>
     <t>End Date, Case</t>
+  </si>
+  <si>
+    <t>Set to migration user</t>
   </si>
 </sst>
 </file>
@@ -481,7 +478,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -534,6 +531,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -751,7 +750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+    <sheetView zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -766,31 +765,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C1" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="11" t="s">
-        <v>84</v>
-      </c>
       <c r="I1" s="11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
@@ -804,53 +803,53 @@
         <v>17</v>
       </c>
       <c r="E2" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="F2" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>86</v>
-      </c>
       <c r="I2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -868,9 +867,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB1000"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S16" sqref="S16"/>
+      <selection pane="bottomLeft" activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -989,7 +988,7 @@
       </c>
       <c r="I2" s="21"/>
       <c r="R2" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1020,14 +1019,14 @@
         <v>25</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="P3" s="21"/>
       <c r="R3" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="S3" s="21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1056,7 +1055,7 @@
       </c>
       <c r="P4" s="21"/>
       <c r="R4" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1084,7 +1083,7 @@
         <v>28</v>
       </c>
       <c r="R5" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1109,7 +1108,7 @@
         <v>0</v>
       </c>
       <c r="R6" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1134,7 +1133,7 @@
       <c r="H7" s="22"/>
       <c r="I7" s="23"/>
       <c r="R7" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1162,7 +1161,7 @@
       <c r="M8" s="9"/>
       <c r="P8" s="21"/>
       <c r="R8" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="S8" s="21"/>
     </row>
@@ -1194,14 +1193,14 @@
         <v>25</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="P9" s="21"/>
       <c r="R9" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="S9" s="21" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1231,7 +1230,7 @@
       </c>
       <c r="I10" s="23"/>
       <c r="R10" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1252,11 +1251,11 @@
       </c>
       <c r="H11" s="22"/>
       <c r="I11" s="21"/>
-      <c r="R11" s="12" t="s">
-        <v>93</v>
+      <c r="R11" s="21" t="s">
+        <v>75</v>
       </c>
       <c r="S11" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:28" ht="99" x14ac:dyDescent="0.2">
@@ -1281,13 +1280,13 @@
         <v>24</v>
       </c>
       <c r="L12" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M12" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="R12" s="12" t="s">
         <v>75</v>
-      </c>
-      <c r="R12" s="12" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1309,7 +1308,7 @@
       <c r="H13" s="22"/>
       <c r="I13" s="21"/>
       <c r="R13" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1331,7 +1330,7 @@
       <c r="H14" s="22"/>
       <c r="I14" s="21"/>
       <c r="R14" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1353,7 +1352,7 @@
       <c r="H15" s="22"/>
       <c r="I15" s="21"/>
       <c r="R15" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1378,10 +1377,10 @@
       <c r="L16" s="7"/>
       <c r="N16" s="9"/>
       <c r="R16" s="9" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="S16" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1403,7 +1402,7 @@
       <c r="H17" s="22"/>
       <c r="I17" s="21"/>
       <c r="R17" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1425,7 +1424,7 @@
       <c r="H18" s="22"/>
       <c r="I18" s="21"/>
       <c r="R18" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1447,7 +1446,7 @@
       <c r="H19" s="22"/>
       <c r="I19" s="21"/>
       <c r="R19" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1471,7 +1470,7 @@
       <c r="J20" s="9"/>
       <c r="L20" s="24"/>
       <c r="R20" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1496,7 +1495,7 @@
       <c r="H21" s="22"/>
       <c r="I21" s="21"/>
       <c r="R21" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1522,14 +1521,14 @@
       <c r="I22" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="O22" s="12">
-        <v>2</v>
+      <c r="O22" s="26">
+        <v>2657</v>
       </c>
       <c r="R22" s="9" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="S22" s="9" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5659,7 +5658,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q8" sqref="Q8"/>
+      <selection pane="bottomLeft" activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5747,7 +5746,7 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>18</v>
@@ -5762,18 +5761,18 @@
         <v>1</v>
       </c>
       <c r="P2" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>20</v>
@@ -5782,41 +5781,41 @@
         <v>0</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="P3" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>57</v>
       </c>
       <c r="E4" s="5" t="b">
         <v>0</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>23</v>
@@ -5825,27 +5824,27 @@
         <v>0</v>
       </c>
       <c r="H5" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="J5" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="P5" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q5" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="P5" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q5" s="6" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>38</v>
@@ -5854,18 +5853,18 @@
         <v>0</v>
       </c>
       <c r="P6" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>23</v>
@@ -5874,24 +5873,24 @@
         <v>0</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P7" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>38</v>
@@ -5903,53 +5902,53 @@
       <c r="J8" s="9"/>
       <c r="L8" s="6"/>
       <c r="P8" s="6" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="Q8" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="99" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E9" s="5" t="b">
         <v>0</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P9" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q9" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>23</v>
@@ -5958,19 +5957,19 @@
         <v>0</v>
       </c>
       <c r="P10" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q10" s="6"/>
     </row>
     <row r="11" spans="1:26" ht="85" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>23</v>
@@ -5979,30 +5978,30 @@
         <v>0</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K11" t="s">
+        <v>74</v>
+      </c>
+      <c r="P11" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="P11" s="6" t="s">
-        <v>76</v>
-      </c>
       <c r="Q11" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>20</v>
@@ -6013,14 +6012,14 @@
       <c r="G12" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="M12">
-        <v>2</v>
+      <c r="M12" s="27">
+        <v>2657</v>
       </c>
       <c r="P12" s="6" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="Q12" s="6" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7532,7 +7531,7 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>18</v>
@@ -7549,13 +7548,13 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>38</v>
@@ -7566,13 +7565,13 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>38</v>
@@ -7583,13 +7582,13 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>38</v>
@@ -7600,13 +7599,13 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>20</v>
@@ -7615,7 +7614,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
IN-924 Set assignee ID to migration user (#468)
* Set assignee_id to migration user for reporting entity

* Set assignees_id to migration user for warnings entity

* Add validation for lodgedby_id (set to migration user)

* Remove deputy_p1_remarks from Warnings spreadsheet
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Reporting.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Reporting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliotsmith/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A83CF8-7E70-3144-A410-B20F86A76D8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26063C6A-E4E9-DD44-820F-F7491F531844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28820" yWindow="460" windowWidth="38380" windowHeight="19440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28820" yWindow="460" windowWidth="38380" windowHeight="19440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="6" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="103">
   <si>
     <t>table_name</t>
   </si>
@@ -184,9 +184,6 @@
   </si>
   <si>
     <t>assignees:id</t>
-  </si>
-  <si>
-    <t>Add migration user</t>
   </si>
   <si>
     <t>annual_report_lodging_details</t>
@@ -323,9 +320,6 @@
     <t>not mapped</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>calculate_duedate</t>
   </si>
   <si>
@@ -351,6 +345,9 @@
   </si>
   <si>
     <t>End Date, Case</t>
+  </si>
+  <si>
+    <t>Set to migration user</t>
   </si>
 </sst>
 </file>
@@ -481,7 +478,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -534,6 +531,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -751,7 +750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+    <sheetView zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -766,31 +765,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C1" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="11" t="s">
-        <v>84</v>
-      </c>
       <c r="I1" s="11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
@@ -804,53 +803,53 @@
         <v>17</v>
       </c>
       <c r="E2" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="F2" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>86</v>
-      </c>
       <c r="I2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -868,9 +867,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB1000"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S16" sqref="S16"/>
+      <selection pane="bottomLeft" activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -989,7 +988,7 @@
       </c>
       <c r="I2" s="21"/>
       <c r="R2" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1020,14 +1019,14 @@
         <v>25</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="P3" s="21"/>
       <c r="R3" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="S3" s="21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1056,7 +1055,7 @@
       </c>
       <c r="P4" s="21"/>
       <c r="R4" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1084,7 +1083,7 @@
         <v>28</v>
       </c>
       <c r="R5" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1109,7 +1108,7 @@
         <v>0</v>
       </c>
       <c r="R6" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1134,7 +1133,7 @@
       <c r="H7" s="22"/>
       <c r="I7" s="23"/>
       <c r="R7" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1162,7 +1161,7 @@
       <c r="M8" s="9"/>
       <c r="P8" s="21"/>
       <c r="R8" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="S8" s="21"/>
     </row>
@@ -1194,14 +1193,14 @@
         <v>25</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="P9" s="21"/>
       <c r="R9" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="S9" s="21" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1231,7 +1230,7 @@
       </c>
       <c r="I10" s="23"/>
       <c r="R10" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1252,11 +1251,11 @@
       </c>
       <c r="H11" s="22"/>
       <c r="I11" s="21"/>
-      <c r="R11" s="12" t="s">
-        <v>93</v>
+      <c r="R11" s="21" t="s">
+        <v>75</v>
       </c>
       <c r="S11" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:28" ht="99" x14ac:dyDescent="0.2">
@@ -1281,13 +1280,13 @@
         <v>24</v>
       </c>
       <c r="L12" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M12" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="R12" s="12" t="s">
         <v>75</v>
-      </c>
-      <c r="R12" s="12" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1309,7 +1308,7 @@
       <c r="H13" s="22"/>
       <c r="I13" s="21"/>
       <c r="R13" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1331,7 +1330,7 @@
       <c r="H14" s="22"/>
       <c r="I14" s="21"/>
       <c r="R14" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1353,7 +1352,7 @@
       <c r="H15" s="22"/>
       <c r="I15" s="21"/>
       <c r="R15" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1378,10 +1377,10 @@
       <c r="L16" s="7"/>
       <c r="N16" s="9"/>
       <c r="R16" s="9" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="S16" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1403,7 +1402,7 @@
       <c r="H17" s="22"/>
       <c r="I17" s="21"/>
       <c r="R17" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1425,7 +1424,7 @@
       <c r="H18" s="22"/>
       <c r="I18" s="21"/>
       <c r="R18" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1447,7 +1446,7 @@
       <c r="H19" s="22"/>
       <c r="I19" s="21"/>
       <c r="R19" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1471,7 +1470,7 @@
       <c r="J20" s="9"/>
       <c r="L20" s="24"/>
       <c r="R20" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1496,7 +1495,7 @@
       <c r="H21" s="22"/>
       <c r="I21" s="21"/>
       <c r="R21" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1522,14 +1521,14 @@
       <c r="I22" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="O22" s="12">
-        <v>2</v>
+      <c r="O22" s="26">
+        <v>2657</v>
       </c>
       <c r="R22" s="9" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="S22" s="9" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5659,7 +5658,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q8" sqref="Q8"/>
+      <selection pane="bottomLeft" activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5747,7 +5746,7 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>18</v>
@@ -5762,18 +5761,18 @@
         <v>1</v>
       </c>
       <c r="P2" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>20</v>
@@ -5782,41 +5781,41 @@
         <v>0</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="P3" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>57</v>
       </c>
       <c r="E4" s="5" t="b">
         <v>0</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>23</v>
@@ -5825,27 +5824,27 @@
         <v>0</v>
       </c>
       <c r="H5" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="J5" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="P5" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q5" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="P5" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q5" s="6" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>38</v>
@@ -5854,18 +5853,18 @@
         <v>0</v>
       </c>
       <c r="P6" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>23</v>
@@ -5874,24 +5873,24 @@
         <v>0</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P7" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>38</v>
@@ -5903,53 +5902,53 @@
       <c r="J8" s="9"/>
       <c r="L8" s="6"/>
       <c r="P8" s="6" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="Q8" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="99" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E9" s="5" t="b">
         <v>0</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P9" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q9" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>23</v>
@@ -5958,19 +5957,19 @@
         <v>0</v>
       </c>
       <c r="P10" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q10" s="6"/>
     </row>
     <row r="11" spans="1:26" ht="85" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>23</v>
@@ -5979,30 +5978,30 @@
         <v>0</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K11" t="s">
+        <v>74</v>
+      </c>
+      <c r="P11" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="P11" s="6" t="s">
-        <v>76</v>
-      </c>
       <c r="Q11" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>20</v>
@@ -6013,14 +6012,14 @@
       <c r="G12" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="M12">
-        <v>2</v>
+      <c r="M12" s="27">
+        <v>2657</v>
       </c>
       <c r="P12" s="6" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="Q12" s="6" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7532,7 +7531,7 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>18</v>
@@ -7549,13 +7548,13 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>38</v>
@@ -7566,13 +7565,13 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>38</v>
@@ -7583,13 +7582,13 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>38</v>
@@ -7600,13 +7599,13 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>20</v>
@@ -7615,7 +7614,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Include reviewdate in reporting migration
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Reporting.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Reporting.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliot.smith/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3ECAD5-4A39-8D46-BF11-6C9016C788EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A936D0-B667-6A48-9D55-0C56CFD0C1FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35840" yWindow="500" windowWidth="38380" windowHeight="19440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="6" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="104">
   <si>
     <t>table_name</t>
   </si>
@@ -348,6 +348,9 @@
   </si>
   <si>
     <t>set_annual_report_logs_status = {"source_cols": ["Rev Stat", "End Date", "Lodge Date", "Rcvd Date", "Rcvd Date1", "Rcvd Date2", "Rcvd Date3", "Rcvd Date4", "Rcvd Date5", "Rcvd Date6", "Review Date", "Next Yr"], "target_cols": ["status", "reviewstatus", "c_rcvd_date"]}</t>
+  </si>
+  <si>
+    <t>Review Date</t>
   </si>
 </sst>
 </file>
@@ -750,7 +753,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+    <sheetView topLeftCell="I1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
       <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
@@ -867,9 +870,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB1000"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R16" sqref="R16"/>
+      <selection pane="bottomLeft" activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1467,10 +1470,14 @@
       </c>
       <c r="H20" s="22"/>
       <c r="I20" s="21"/>
-      <c r="J20" s="9"/>
-      <c r="L20" s="24"/>
+      <c r="J20" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="L20" s="24" t="s">
+        <v>103</v>
+      </c>
       <c r="R20" s="9" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
IN-1150 Reporting reviewdate (#562)
* Include reviewdate in reporting migration

* Update reporting validation for reviewdate

* Add API test for reviewdate

Was a 10 minute job, so did included it.
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Reporting.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Reporting.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliot.smith/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3ECAD5-4A39-8D46-BF11-6C9016C788EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A936D0-B667-6A48-9D55-0C56CFD0C1FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35840" yWindow="500" windowWidth="38380" windowHeight="19440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="6" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="104">
   <si>
     <t>table_name</t>
   </si>
@@ -348,6 +348,9 @@
   </si>
   <si>
     <t>set_annual_report_logs_status = {"source_cols": ["Rev Stat", "End Date", "Lodge Date", "Rcvd Date", "Rcvd Date1", "Rcvd Date2", "Rcvd Date3", "Rcvd Date4", "Rcvd Date5", "Rcvd Date6", "Review Date", "Next Yr"], "target_cols": ["status", "reviewstatus", "c_rcvd_date"]}</t>
+  </si>
+  <si>
+    <t>Review Date</t>
   </si>
 </sst>
 </file>
@@ -750,7 +753,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+    <sheetView topLeftCell="I1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
       <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
@@ -867,9 +870,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB1000"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R16" sqref="R16"/>
+      <selection pane="bottomLeft" activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1467,10 +1470,14 @@
       </c>
       <c r="H20" s="22"/>
       <c r="I20" s="21"/>
-      <c r="J20" s="9"/>
-      <c r="L20" s="24"/>
+      <c r="J20" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="L20" s="24" t="s">
+        <v>103</v>
+      </c>
       <c r="R20" s="9" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add fields needed for additional dates in annual_report_logs
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Reporting.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Reporting.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliot.smith/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A936D0-B667-6A48-9D55-0C56CFD0C1FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDEB12D1-857B-9C44-8C40-452CCBE2C914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -285,9 +285,6 @@
     <t>data</t>
   </si>
   <si>
-    <t>Case</t>
-  </si>
-  <si>
     <t>account</t>
   </si>
   <si>
@@ -351,6 +348,9 @@
   </si>
   <si>
     <t>Review Date</t>
+  </si>
+  <si>
+    <t>Case, Further1, Further2, Further3, Further4, Further5, Further6, Further Date1, Further Date2, Further Date3, Further Date4, Further Date6, Further Date6.1</t>
   </si>
 </sst>
 </file>
@@ -753,8 +753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+    <sheetView topLeftCell="G1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -792,7 +792,7 @@
         <v>83</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
@@ -809,13 +809,13 @@
         <v>84</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="I2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
@@ -832,13 +832,13 @@
         <v>84</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
@@ -868,11 +868,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AB1000"/>
+  <dimension ref="A1:AB997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R20" sqref="R20"/>
+      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -991,7 +991,7 @@
       </c>
       <c r="I2" s="21"/>
       <c r="R2" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1022,14 +1022,14 @@
         <v>25</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P3" s="21"/>
       <c r="R3" s="12" t="s">
         <v>75</v>
       </c>
       <c r="S3" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1136,7 +1136,7 @@
       <c r="H7" s="22"/>
       <c r="I7" s="23"/>
       <c r="R7" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1164,7 +1164,7 @@
       <c r="M8" s="9"/>
       <c r="P8" s="21"/>
       <c r="R8" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="S8" s="21"/>
     </row>
@@ -1196,14 +1196,14 @@
         <v>25</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="P9" s="21"/>
       <c r="R9" s="12" t="s">
         <v>75</v>
       </c>
       <c r="S9" s="21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1233,7 +1233,7 @@
       </c>
       <c r="I10" s="23"/>
       <c r="R10" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1258,7 +1258,7 @@
         <v>75</v>
       </c>
       <c r="S11" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:28" ht="99" x14ac:dyDescent="0.2">
@@ -1283,7 +1283,7 @@
         <v>24</v>
       </c>
       <c r="L12" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M12" s="12" t="s">
         <v>74</v>
@@ -1311,7 +1311,7 @@
       <c r="H13" s="22"/>
       <c r="I13" s="21"/>
       <c r="R13" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1333,7 +1333,7 @@
       <c r="H14" s="22"/>
       <c r="I14" s="21"/>
       <c r="R14" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1355,7 +1355,7 @@
       <c r="H15" s="22"/>
       <c r="I15" s="21"/>
       <c r="R15" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1383,7 +1383,7 @@
         <v>75</v>
       </c>
       <c r="S16" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1405,7 +1405,7 @@
       <c r="H17" s="22"/>
       <c r="I17" s="21"/>
       <c r="R17" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1427,7 +1427,7 @@
       <c r="H18" s="22"/>
       <c r="I18" s="21"/>
       <c r="R18" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1449,7 +1449,7 @@
       <c r="H19" s="22"/>
       <c r="I19" s="21"/>
       <c r="R19" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1474,7 +1474,7 @@
         <v>24</v>
       </c>
       <c r="L20" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="R20" s="9" t="s">
         <v>75</v>
@@ -1502,7 +1502,7 @@
       <c r="H21" s="22"/>
       <c r="I21" s="21"/>
       <c r="R21" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1535,7 +1535,7 @@
         <v>75</v>
       </c>
       <c r="S22" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2514,17 +2514,14 @@
       <c r="I217" s="21"/>
     </row>
     <row r="218" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B218" s="8"/>
       <c r="H218" s="22"/>
       <c r="I218" s="21"/>
     </row>
     <row r="219" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B219" s="8"/>
       <c r="H219" s="22"/>
       <c r="I219" s="21"/>
     </row>
     <row r="220" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B220" s="8"/>
       <c r="H220" s="22"/>
       <c r="I220" s="21"/>
     </row>
@@ -5635,18 +5632,6 @@
     <row r="997" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="H997" s="22"/>
       <c r="I997" s="21"/>
-    </row>
-    <row r="998" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="H998" s="22"/>
-      <c r="I998" s="21"/>
-    </row>
-    <row r="999" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="H999" s="22"/>
-      <c r="I999" s="21"/>
-    </row>
-    <row r="1000" spans="8:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="H1000" s="22"/>
-      <c r="I1000" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -5768,7 +5753,7 @@
         <v>1</v>
       </c>
       <c r="P2" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5791,7 +5776,7 @@
         <v>54</v>
       </c>
       <c r="P3" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5811,7 +5796,7 @@
         <v>0</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5860,7 +5845,7 @@
         <v>0</v>
       </c>
       <c r="P6" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5912,7 +5897,7 @@
         <v>75</v>
       </c>
       <c r="Q8" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="99" x14ac:dyDescent="0.2">
@@ -5935,16 +5920,16 @@
         <v>58</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="P9" s="6" t="s">
         <v>75</v>
       </c>
       <c r="Q9" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5964,7 +5949,7 @@
         <v>0</v>
       </c>
       <c r="P10" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q10" s="6"/>
     </row>
@@ -5988,7 +5973,7 @@
         <v>58</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K11" t="s">
         <v>74</v>
@@ -5997,7 +5982,7 @@
         <v>75</v>
       </c>
       <c r="Q11" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6026,7 +6011,7 @@
         <v>75</v>
       </c>
       <c r="Q12" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Move reporting additional dates mapping to correct tab of spreadsheet
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Reporting.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Reporting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliot.smith/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDEB12D1-857B-9C44-8C40-452CCBE2C914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947C90E5-1D97-1B47-8B64-06E076369A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="6" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="101">
   <si>
     <t>table_name</t>
   </si>
@@ -205,12 +205,6 @@
   </si>
   <si>
     <t>ACCOUNT</t>
-  </si>
-  <si>
-    <t>Followup Date</t>
-  </si>
-  <si>
-    <t>Only Latest Reporting Period</t>
   </si>
   <si>
     <t>reasonfordetermination</t>
@@ -297,20 +291,9 @@
 Rcvd Date6</t>
   </si>
   <si>
-    <t>Sent1
-Sent2
-Sent3
-Sent4
-Sent5
-Sent6</t>
-  </si>
-  <si>
     <t>is_at_least_one_set</t>
   </si>
   <si>
-    <t>Specified in IN-748; set to the latest date in the Sent* columns</t>
-  </si>
-  <si>
     <t>Specified in IN-748; true if at least one of the Rcvd Date* columns has a non-empty value</t>
   </si>
   <si>
@@ -338,9 +321,6 @@
     <t>set_annual_report_lodging_details_status = {"source_cols": ["Rev Stat", "Lodge Date", "Rcvd Date", "Rcvd Date1", "Rcvd Date2", "Rcvd Date3", "Rcvd Date4", "Rcvd Date5", "Rcvd Date6", "Review Date", "Revise Date", "Further Code", "Sent1", "Sent2", "Sent3", "Sent4", "Sent5", "Sent6", "Followup Date"], "target_cols": ["lodgedstatus"]}</t>
   </si>
   <si>
-    <t>End Date, Case</t>
-  </si>
-  <si>
     <t>Set to migration user</t>
   </si>
   <si>
@@ -350,7 +330,13 @@
     <t>Review Date</t>
   </si>
   <si>
-    <t>Case, Further1, Further2, Further3, Further4, Further5, Further6, Further Date1, Further Date2, Further Date3, Further Date4, Further Date6, Further Date6.1</t>
+    <t>Case</t>
+  </si>
+  <si>
+    <t>End Date, Case, Further1, Further2, Further3, Further4, Further5, Further6, Further Date1, Further Date2, Further Date3, Further Date4, Further Date6, Further Date6.1</t>
+  </si>
+  <si>
+    <t>Specified in IN-1152</t>
   </si>
 </sst>
 </file>
@@ -753,8 +739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -768,31 +754,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="D1" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="G1" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>83</v>
-      </c>
       <c r="I1" s="11" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
@@ -806,16 +792,16 @@
         <v>17</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="I2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
@@ -829,30 +815,30 @@
         <v>52</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H3" t="s">
         <v>99</v>
       </c>
       <c r="I3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -870,7 +856,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
     </sheetView>
@@ -991,7 +977,7 @@
       </c>
       <c r="I2" s="21"/>
       <c r="R2" s="12" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1022,14 +1008,14 @@
         <v>25</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="P3" s="21"/>
       <c r="R3" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="S3" s="21" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1058,7 +1044,7 @@
       </c>
       <c r="P4" s="21"/>
       <c r="R4" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1086,7 +1072,7 @@
         <v>28</v>
       </c>
       <c r="R5" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1111,7 +1097,7 @@
         <v>0</v>
       </c>
       <c r="R6" s="21" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1136,7 +1122,7 @@
       <c r="H7" s="22"/>
       <c r="I7" s="23"/>
       <c r="R7" s="12" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1164,7 +1150,7 @@
       <c r="M8" s="9"/>
       <c r="P8" s="21"/>
       <c r="R8" s="12" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="S8" s="21"/>
     </row>
@@ -1196,14 +1182,14 @@
         <v>25</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="P9" s="21"/>
       <c r="R9" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="S9" s="21" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1233,7 +1219,7 @@
       </c>
       <c r="I10" s="23"/>
       <c r="R10" s="12" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1255,10 +1241,10 @@
       <c r="H11" s="22"/>
       <c r="I11" s="21"/>
       <c r="R11" s="21" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="S11" s="12" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:28" ht="99" x14ac:dyDescent="0.2">
@@ -1283,13 +1269,13 @@
         <v>24</v>
       </c>
       <c r="L12" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M12" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="R12" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1311,7 +1297,7 @@
       <c r="H13" s="22"/>
       <c r="I13" s="21"/>
       <c r="R13" s="12" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1333,7 +1319,7 @@
       <c r="H14" s="22"/>
       <c r="I14" s="21"/>
       <c r="R14" s="12" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1355,7 +1341,7 @@
       <c r="H15" s="22"/>
       <c r="I15" s="21"/>
       <c r="R15" s="12" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1380,10 +1366,10 @@
       <c r="L16" s="7"/>
       <c r="N16" s="9"/>
       <c r="R16" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="S16" s="9" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1405,7 +1391,7 @@
       <c r="H17" s="22"/>
       <c r="I17" s="21"/>
       <c r="R17" s="9" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1427,7 +1413,7 @@
       <c r="H18" s="22"/>
       <c r="I18" s="21"/>
       <c r="R18" s="9" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1449,7 +1435,7 @@
       <c r="H19" s="22"/>
       <c r="I19" s="21"/>
       <c r="R19" s="9" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1474,10 +1460,10 @@
         <v>24</v>
       </c>
       <c r="L20" s="24" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="R20" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1502,7 +1488,7 @@
       <c r="H21" s="22"/>
       <c r="I21" s="21"/>
       <c r="R21" s="9" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1532,10 +1518,10 @@
         <v>2657</v>
       </c>
       <c r="R22" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="S22" s="9" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5648,9 +5634,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P9" sqref="P9"/>
+      <selection pane="bottomLeft" activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5753,7 +5739,7 @@
         <v>1</v>
       </c>
       <c r="P2" s="13" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5776,7 +5762,7 @@
         <v>54</v>
       </c>
       <c r="P3" s="13" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5796,7 +5782,7 @@
         <v>0</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5815,17 +5801,13 @@
       <c r="E5" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H5" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>59</v>
-      </c>
+      <c r="H5" s="9"/>
+      <c r="J5" s="9"/>
       <c r="P5" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="Q5" s="6" t="s">
-        <v>60</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5836,7 +5818,7 @@
         <v>18</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>38</v>
@@ -5845,7 +5827,7 @@
         <v>0</v>
       </c>
       <c r="P6" s="6" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5856,7 +5838,7 @@
         <v>18</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>23</v>
@@ -5868,10 +5850,10 @@
         <v>58</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="P7" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5882,7 +5864,7 @@
         <v>18</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>38</v>
@@ -5894,10 +5876,10 @@
       <c r="J8" s="9"/>
       <c r="L8" s="6"/>
       <c r="P8" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="Q8" s="6" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="99" x14ac:dyDescent="0.2">
@@ -5908,7 +5890,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>56</v>
@@ -5920,16 +5902,16 @@
         <v>58</v>
       </c>
       <c r="J9" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="K9" t="s">
+        <v>85</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q9" s="6" t="s">
         <v>86</v>
-      </c>
-      <c r="K9" t="s">
-        <v>88</v>
-      </c>
-      <c r="P9" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q9" s="6" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5940,7 +5922,7 @@
         <v>18</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>23</v>
@@ -5949,11 +5931,13 @@
         <v>0</v>
       </c>
       <c r="P10" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q10" s="6"/>
-    </row>
-    <row r="11" spans="1:26" ht="85" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+      <c r="Q10" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>52</v>
       </c>
@@ -5961,7 +5945,7 @@
         <v>18</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>23</v>
@@ -5969,20 +5953,13 @@
       <c r="E11" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H11" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="J11" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="K11" t="s">
-        <v>74</v>
-      </c>
+      <c r="H11" s="6"/>
+      <c r="J11" s="10"/>
       <c r="P11" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="Q11" s="6" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5993,7 +5970,7 @@
         <v>18</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>20</v>
@@ -6008,10 +5985,10 @@
         <v>2657</v>
       </c>
       <c r="P12" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="Q12" s="6" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7523,7 +7500,7 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>18</v>
@@ -7540,13 +7517,13 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>38</v>
@@ -7557,13 +7534,13 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>38</v>
@@ -7574,13 +7551,13 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>38</v>
@@ -7591,13 +7568,13 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Update report receiveddate mapping
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Reporting.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Reporting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliot.smith/projects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947C90E5-1D97-1B47-8B64-06E076369A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59110B3A-793A-F74B-B060-163AC978B98F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="6" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="102">
   <si>
     <t>table_name</t>
   </si>
@@ -244,9 +244,6 @@
   </si>
   <si>
     <t>annualreport_id</t>
-  </si>
-  <si>
-    <t>get_max_col</t>
   </si>
   <si>
     <t>yes</t>
@@ -337,6 +334,13 @@
   </si>
   <si>
     <t>Specified in IN-1152</t>
+  </si>
+  <si>
+    <t>coalesce</t>
+  </si>
+  <si>
+    <t>Rcvd Date
+Lodge Date</t>
   </si>
 </sst>
 </file>
@@ -754,31 +758,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C1" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="H1" s="11" t="s">
-        <v>81</v>
-      </c>
       <c r="I1" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
@@ -792,16 +796,16 @@
         <v>17</v>
       </c>
       <c r="E2" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="F2" s="13" t="s">
-        <v>83</v>
-      </c>
       <c r="H2" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
@@ -815,16 +819,16 @@
         <v>52</v>
       </c>
       <c r="E3" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="F3" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="F3" s="13" t="s">
-        <v>83</v>
-      </c>
       <c r="H3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
@@ -838,7 +842,7 @@
         <v>67</v>
       </c>
       <c r="E4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -856,9 +860,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
+      <selection pane="bottomLeft" activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -977,7 +981,7 @@
       </c>
       <c r="I2" s="21"/>
       <c r="R2" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1008,14 +1012,14 @@
         <v>25</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="P3" s="21"/>
       <c r="R3" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="S3" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1044,7 +1048,7 @@
       </c>
       <c r="P4" s="21"/>
       <c r="R4" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1072,7 +1076,7 @@
         <v>28</v>
       </c>
       <c r="R5" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1097,7 +1101,7 @@
         <v>0</v>
       </c>
       <c r="R6" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1122,7 +1126,7 @@
       <c r="H7" s="22"/>
       <c r="I7" s="23"/>
       <c r="R7" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1150,7 +1154,7 @@
       <c r="M8" s="9"/>
       <c r="P8" s="21"/>
       <c r="R8" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="S8" s="21"/>
     </row>
@@ -1182,14 +1186,14 @@
         <v>25</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P9" s="21"/>
       <c r="R9" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="S9" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1219,7 +1223,7 @@
       </c>
       <c r="I10" s="23"/>
       <c r="R10" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1241,13 +1245,13 @@
       <c r="H11" s="22"/>
       <c r="I11" s="21"/>
       <c r="R11" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="S11" s="12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="12" spans="1:28" ht="99" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" ht="29" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>17</v>
       </c>
@@ -1269,13 +1273,13 @@
         <v>24</v>
       </c>
       <c r="L12" s="10" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="M12" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="R12" s="12" t="s">
         <v>72</v>
-      </c>
-      <c r="R12" s="12" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1297,7 +1301,7 @@
       <c r="H13" s="22"/>
       <c r="I13" s="21"/>
       <c r="R13" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1319,7 +1323,7 @@
       <c r="H14" s="22"/>
       <c r="I14" s="21"/>
       <c r="R14" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1341,7 +1345,7 @@
       <c r="H15" s="22"/>
       <c r="I15" s="21"/>
       <c r="R15" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1366,10 +1370,10 @@
       <c r="L16" s="7"/>
       <c r="N16" s="9"/>
       <c r="R16" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="S16" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1391,7 +1395,7 @@
       <c r="H17" s="22"/>
       <c r="I17" s="21"/>
       <c r="R17" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1413,7 +1417,7 @@
       <c r="H18" s="22"/>
       <c r="I18" s="21"/>
       <c r="R18" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1435,7 +1439,7 @@
       <c r="H19" s="22"/>
       <c r="I19" s="21"/>
       <c r="R19" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1460,10 +1464,10 @@
         <v>24</v>
       </c>
       <c r="L20" s="24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="R20" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1488,7 +1492,7 @@
       <c r="H21" s="22"/>
       <c r="I21" s="21"/>
       <c r="R21" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1518,10 +1522,10 @@
         <v>2657</v>
       </c>
       <c r="R22" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="S22" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5634,9 +5638,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q11" sqref="Q11"/>
+      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5739,7 +5743,7 @@
         <v>1</v>
       </c>
       <c r="P2" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5762,7 +5766,7 @@
         <v>54</v>
       </c>
       <c r="P3" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5782,7 +5786,7 @@
         <v>0</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5804,10 +5808,10 @@
       <c r="H5" s="9"/>
       <c r="J5" s="9"/>
       <c r="P5" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q5" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5827,7 +5831,7 @@
         <v>0</v>
       </c>
       <c r="P6" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5853,7 +5857,7 @@
         <v>61</v>
       </c>
       <c r="P7" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5876,10 +5880,10 @@
       <c r="J8" s="9"/>
       <c r="L8" s="6"/>
       <c r="P8" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q8" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="99" x14ac:dyDescent="0.2">
@@ -5902,16 +5906,16 @@
         <v>58</v>
       </c>
       <c r="J9" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="K9" t="s">
         <v>84</v>
       </c>
-      <c r="K9" t="s">
+      <c r="P9" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q9" s="6" t="s">
         <v>85</v>
-      </c>
-      <c r="P9" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q9" s="6" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5931,10 +5935,10 @@
         <v>0</v>
       </c>
       <c r="P10" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q10" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
@@ -5956,10 +5960,10 @@
       <c r="H11" s="6"/>
       <c r="J11" s="10"/>
       <c r="P11" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q11" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5985,10 +5989,10 @@
         <v>2657</v>
       </c>
       <c r="P12" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q12" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>